<commit_message>
Added a new csv with A and GS
</commit_message>
<xml_diff>
--- a/Data/ACi fitting that corresponds to R library plantecophys.xlsx
+++ b/Data/ACi fitting that corresponds to R library plantecophys.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\GitHub\CO2-effects-on-geophytes\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E417AAD0-20C1-491A-A98E-71D362034423}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41308E8E-7C6B-4E82-8B9F-A3E7A1A39B13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ACidata" sheetId="1" r:id="rId1"/>
@@ -11467,8 +11467,8 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I560"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B535" sqref="B535"/>
+    <sheetView tabSelected="1" topLeftCell="A406" workbookViewId="0">
+      <selection sqref="A1:I219"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -17827,7 +17827,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="220" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="220" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A220">
         <v>2</v>
       </c>
@@ -17856,7 +17856,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="221" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="221" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A221">
         <v>2</v>
       </c>
@@ -17885,7 +17885,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="222" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="222" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A222">
         <v>2</v>
       </c>
@@ -17914,7 +17914,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="223" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="223" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A223">
         <v>2</v>
       </c>
@@ -17943,7 +17943,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="224" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="224" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A224">
         <v>2</v>
       </c>
@@ -17972,7 +17972,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="225" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="225" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A225">
         <v>2</v>
       </c>
@@ -18001,7 +18001,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="226" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="226" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A226">
         <v>2</v>
       </c>
@@ -18030,7 +18030,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="227" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="227" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A227">
         <v>2</v>
       </c>
@@ -18059,7 +18059,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="228" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="228" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A228">
         <v>2</v>
       </c>
@@ -18088,7 +18088,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="229" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="229" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A229">
         <v>2</v>
       </c>
@@ -18117,7 +18117,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="230" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="230" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A230">
         <v>2</v>
       </c>
@@ -18146,7 +18146,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="231" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="231" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A231">
         <v>2</v>
       </c>
@@ -18175,7 +18175,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="232" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="232" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A232">
         <v>2</v>
       </c>
@@ -18204,7 +18204,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="233" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="233" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A233">
         <v>2</v>
       </c>
@@ -18233,7 +18233,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="234" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="234" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A234">
         <v>2</v>
       </c>
@@ -18262,7 +18262,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="235" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="235" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A235">
         <v>2</v>
       </c>
@@ -18291,7 +18291,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="236" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="236" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A236">
         <v>2</v>
       </c>
@@ -18320,7 +18320,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="237" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="237" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A237">
         <v>2</v>
       </c>
@@ -18349,7 +18349,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="238" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="238" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A238">
         <v>2</v>
       </c>
@@ -18378,7 +18378,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="239" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="239" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A239">
         <v>2</v>
       </c>
@@ -18407,7 +18407,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="240" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="240" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A240">
         <v>2</v>
       </c>
@@ -18436,7 +18436,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="241" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="241" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A241">
         <v>2</v>
       </c>
@@ -18465,7 +18465,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="242" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="242" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A242">
         <v>2</v>
       </c>
@@ -18494,7 +18494,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="243" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="243" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A243">
         <v>2</v>
       </c>
@@ -18523,7 +18523,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="244" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="244" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A244">
         <v>2</v>
       </c>
@@ -18552,7 +18552,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="245" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="245" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A245">
         <v>2</v>
       </c>
@@ -18581,7 +18581,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="246" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="246" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A246">
         <v>2</v>
       </c>
@@ -18610,7 +18610,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="247" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="247" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A247">
         <v>2</v>
       </c>
@@ -18639,7 +18639,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="248" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="248" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A248">
         <v>2</v>
       </c>
@@ -18668,7 +18668,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="249" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="249" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A249">
         <v>2</v>
       </c>
@@ -18697,7 +18697,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="250" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="250" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A250">
         <v>2</v>
       </c>
@@ -18726,7 +18726,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="251" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="251" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A251">
         <v>2</v>
       </c>
@@ -18755,7 +18755,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="252" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="252" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A252">
         <v>2</v>
       </c>
@@ -18784,7 +18784,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="253" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="253" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A253">
         <v>2</v>
       </c>
@@ -18813,7 +18813,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="254" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="254" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A254">
         <v>2</v>
       </c>
@@ -18842,7 +18842,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="255" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="255" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A255">
         <v>2</v>
       </c>
@@ -18871,7 +18871,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="256" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="256" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A256">
         <v>2</v>
       </c>
@@ -18900,7 +18900,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="257" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="257" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A257">
         <v>2</v>
       </c>
@@ -18929,7 +18929,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="258" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="258" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A258">
         <v>2</v>
       </c>
@@ -18958,7 +18958,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="259" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="259" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A259">
         <v>2</v>
       </c>
@@ -18987,7 +18987,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="260" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="260" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A260">
         <v>2</v>
       </c>
@@ -19016,7 +19016,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="261" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="261" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A261">
         <v>2</v>
       </c>
@@ -19045,7 +19045,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="262" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="262" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A262">
         <v>2</v>
       </c>
@@ -19074,7 +19074,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="263" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="263" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A263">
         <v>2</v>
       </c>
@@ -19103,7 +19103,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="264" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="264" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A264">
         <v>2</v>
       </c>
@@ -19132,7 +19132,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="265" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="265" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A265">
         <v>2</v>
       </c>
@@ -19161,7 +19161,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="266" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="266" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A266">
         <v>2</v>
       </c>
@@ -19190,7 +19190,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="267" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="267" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A267">
         <v>2</v>
       </c>
@@ -19219,7 +19219,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="268" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="268" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A268">
         <v>2</v>
       </c>
@@ -19248,7 +19248,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="269" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="269" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A269">
         <v>2</v>
       </c>
@@ -19277,7 +19277,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="270" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="270" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A270">
         <v>2</v>
       </c>
@@ -19306,7 +19306,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="271" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="271" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A271">
         <v>2</v>
       </c>
@@ -19335,7 +19335,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="272" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="272" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A272">
         <v>2</v>
       </c>
@@ -19364,7 +19364,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="273" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="273" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A273">
         <v>2</v>
       </c>
@@ -19393,7 +19393,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="274" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="274" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A274">
         <v>2</v>
       </c>
@@ -19422,7 +19422,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="275" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="275" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A275">
         <v>2</v>
       </c>
@@ -19451,7 +19451,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="276" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="276" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A276">
         <v>2</v>
       </c>
@@ -19480,7 +19480,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="277" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="277" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A277">
         <v>2</v>
       </c>
@@ -19509,7 +19509,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="278" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="278" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A278">
         <v>2</v>
       </c>
@@ -19538,7 +19538,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="279" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="279" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A279">
         <v>2</v>
       </c>
@@ -19567,7 +19567,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="280" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="280" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A280">
         <v>2</v>
       </c>
@@ -19596,7 +19596,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="281" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="281" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A281">
         <v>2</v>
       </c>
@@ -19625,7 +19625,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="282" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="282" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A282">
         <v>2</v>
       </c>
@@ -19654,7 +19654,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="283" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="283" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A283">
         <v>2</v>
       </c>
@@ -19683,7 +19683,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="284" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="284" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A284">
         <v>2</v>
       </c>
@@ -19712,7 +19712,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="285" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="285" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A285">
         <v>2</v>
       </c>
@@ -19741,7 +19741,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="286" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="286" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A286">
         <v>2</v>
       </c>
@@ -19770,7 +19770,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="287" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="287" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A287">
         <v>2</v>
       </c>
@@ -19799,7 +19799,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="288" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="288" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A288">
         <v>2</v>
       </c>
@@ -19828,7 +19828,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="289" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="289" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A289">
         <v>2</v>
       </c>
@@ -19857,7 +19857,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="290" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="290" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A290">
         <v>2</v>
       </c>
@@ -19886,7 +19886,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="291" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="291" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A291">
         <v>2</v>
       </c>
@@ -19915,7 +19915,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="292" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="292" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A292">
         <v>2</v>
       </c>
@@ -19944,7 +19944,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="293" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="293" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A293">
         <v>2</v>
       </c>
@@ -19973,7 +19973,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="294" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="294" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A294">
         <v>2</v>
       </c>
@@ -20002,7 +20002,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="295" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="295" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A295">
         <v>2</v>
       </c>
@@ -20031,7 +20031,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="296" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="296" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A296">
         <v>2</v>
       </c>
@@ -20060,7 +20060,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="297" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="297" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A297">
         <v>2</v>
       </c>
@@ -20089,7 +20089,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="298" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="298" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A298">
         <v>2</v>
       </c>
@@ -20118,7 +20118,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="299" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="299" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A299">
         <v>2</v>
       </c>
@@ -20147,7 +20147,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="300" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="300" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A300">
         <v>2</v>
       </c>
@@ -20176,7 +20176,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="301" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="301" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A301">
         <v>2</v>
       </c>
@@ -20205,7 +20205,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="302" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="302" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A302">
         <v>2</v>
       </c>
@@ -20234,7 +20234,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="303" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="303" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A303">
         <v>2</v>
       </c>
@@ -20263,7 +20263,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="304" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="304" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A304">
         <v>2</v>
       </c>
@@ -20292,7 +20292,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="305" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="305" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A305">
         <v>2</v>
       </c>
@@ -20321,7 +20321,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="306" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="306" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A306">
         <v>2</v>
       </c>
@@ -20350,7 +20350,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="307" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="307" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A307">
         <v>2</v>
       </c>
@@ -20379,7 +20379,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="308" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="308" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A308">
         <v>2</v>
       </c>
@@ -20408,7 +20408,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="309" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="309" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A309">
         <v>2</v>
       </c>
@@ -20437,7 +20437,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="310" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="310" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A310">
         <v>2</v>
       </c>
@@ -20466,7 +20466,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="311" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="311" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A311">
         <v>2</v>
       </c>
@@ -20495,7 +20495,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="312" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="312" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A312">
         <v>2</v>
       </c>
@@ -20524,7 +20524,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="313" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="313" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A313">
         <v>2</v>
       </c>
@@ -20553,7 +20553,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="314" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="314" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A314">
         <v>2</v>
       </c>
@@ -20582,7 +20582,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="315" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="315" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A315">
         <v>2</v>
       </c>
@@ -20611,7 +20611,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="316" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="316" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A316">
         <v>2</v>
       </c>
@@ -20640,7 +20640,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="317" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="317" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A317">
         <v>2</v>
       </c>
@@ -20669,7 +20669,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="318" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="318" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A318">
         <v>2</v>
       </c>
@@ -20698,7 +20698,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="319" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="319" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A319">
         <v>2</v>
       </c>
@@ -20727,7 +20727,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="320" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="320" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A320">
         <v>2</v>
       </c>
@@ -20756,7 +20756,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="321" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="321" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A321">
         <v>2</v>
       </c>
@@ -20785,7 +20785,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="322" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="322" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A322">
         <v>2</v>
       </c>
@@ -20814,7 +20814,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="323" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="323" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A323">
         <v>2</v>
       </c>
@@ -20843,7 +20843,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="324" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="324" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A324">
         <v>2</v>
       </c>
@@ -20872,7 +20872,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="325" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="325" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A325">
         <v>2</v>
       </c>
@@ -20901,7 +20901,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="326" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="326" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A326">
         <v>2</v>
       </c>
@@ -20930,7 +20930,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="327" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="327" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A327">
         <v>2</v>
       </c>
@@ -20959,7 +20959,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="328" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="328" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A328">
         <v>2</v>
       </c>
@@ -20988,7 +20988,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="329" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="329" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A329">
         <v>2</v>
       </c>
@@ -21017,7 +21017,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="330" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="330" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A330">
         <v>2</v>
       </c>
@@ -21046,7 +21046,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="331" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="331" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A331">
         <v>2</v>
       </c>
@@ -21075,7 +21075,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="332" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="332" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A332">
         <v>2</v>
       </c>
@@ -21104,7 +21104,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="333" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="333" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A333">
         <v>2</v>
       </c>
@@ -21133,7 +21133,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="334" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="334" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A334">
         <v>2</v>
       </c>
@@ -21162,7 +21162,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="335" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="335" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A335">
         <v>2</v>
       </c>
@@ -21191,7 +21191,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="336" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="336" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A336">
         <v>2</v>
       </c>
@@ -21220,7 +21220,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="337" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="337" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A337">
         <v>2</v>
       </c>
@@ -21249,7 +21249,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="338" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="338" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A338">
         <v>2</v>
       </c>
@@ -21278,7 +21278,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="339" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="339" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A339">
         <v>2</v>
       </c>
@@ -21307,7 +21307,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="340" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="340" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A340">
         <v>2</v>
       </c>
@@ -21336,7 +21336,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="341" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="341" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A341">
         <v>2</v>
       </c>
@@ -21365,7 +21365,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="342" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="342" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A342">
         <v>2</v>
       </c>
@@ -21394,7 +21394,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="343" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="343" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A343">
         <v>2</v>
       </c>
@@ -21423,7 +21423,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="344" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="344" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A344">
         <v>2</v>
       </c>
@@ -21452,7 +21452,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="345" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="345" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A345">
         <v>2</v>
       </c>
@@ -21481,7 +21481,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="346" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="346" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A346">
         <v>2</v>
       </c>
@@ -21510,7 +21510,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="347" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="347" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A347">
         <v>2</v>
       </c>
@@ -21539,7 +21539,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="348" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="348" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A348">
         <v>2</v>
       </c>
@@ -21568,7 +21568,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="349" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="349" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A349">
         <v>2</v>
       </c>
@@ -21597,7 +21597,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="350" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="350" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A350">
         <v>2</v>
       </c>
@@ -21626,7 +21626,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="351" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="351" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A351">
         <v>2</v>
       </c>
@@ -21655,7 +21655,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="352" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="352" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A352">
         <v>2</v>
       </c>
@@ -21684,7 +21684,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="353" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="353" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A353">
         <v>2</v>
       </c>
@@ -21713,7 +21713,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="354" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="354" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A354">
         <v>2</v>
       </c>
@@ -21742,7 +21742,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="355" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="355" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A355">
         <v>2</v>
       </c>
@@ -21771,7 +21771,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="356" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="356" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A356">
         <v>2</v>
       </c>
@@ -21800,7 +21800,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="357" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="357" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A357">
         <v>2</v>
       </c>
@@ -21829,7 +21829,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="358" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="358" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A358">
         <v>2</v>
       </c>
@@ -21858,7 +21858,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="359" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="359" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A359">
         <v>2</v>
       </c>
@@ -21887,7 +21887,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="360" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="360" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A360">
         <v>2</v>
       </c>
@@ -21916,7 +21916,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="361" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="361" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A361">
         <v>2</v>
       </c>
@@ -21945,7 +21945,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="362" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="362" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A362">
         <v>2</v>
       </c>
@@ -21974,7 +21974,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="363" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="363" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A363">
         <v>2</v>
       </c>
@@ -22003,7 +22003,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="364" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="364" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A364">
         <v>2</v>
       </c>
@@ -22032,7 +22032,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="365" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="365" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A365">
         <v>2</v>
       </c>
@@ -22061,7 +22061,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="366" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="366" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A366">
         <v>2</v>
       </c>
@@ -22090,7 +22090,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="367" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="367" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A367">
         <v>2</v>
       </c>
@@ -22119,7 +22119,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="368" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="368" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A368">
         <v>2</v>
       </c>
@@ -22148,7 +22148,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="369" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="369" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A369">
         <v>2</v>
       </c>
@@ -22177,7 +22177,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="370" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="370" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A370">
         <v>2</v>
       </c>
@@ -22206,7 +22206,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="371" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="371" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A371">
         <v>2</v>
       </c>
@@ -22235,7 +22235,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="372" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="372" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A372">
         <v>2</v>
       </c>
@@ -22264,7 +22264,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="373" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="373" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A373">
         <v>2</v>
       </c>
@@ -22293,7 +22293,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="374" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="374" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A374">
         <v>2</v>
       </c>
@@ -22322,7 +22322,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="375" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="375" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A375">
         <v>2</v>
       </c>
@@ -22351,7 +22351,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="376" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="376" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A376">
         <v>2</v>
       </c>
@@ -22380,7 +22380,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="377" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="377" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A377">
         <v>2</v>
       </c>
@@ -22409,7 +22409,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="378" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="378" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A378">
         <v>2</v>
       </c>
@@ -22438,7 +22438,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="379" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="379" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A379">
         <v>2</v>
       </c>
@@ -22467,7 +22467,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="380" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="380" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A380">
         <v>2</v>
       </c>
@@ -22496,7 +22496,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="381" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="381" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A381">
         <v>2</v>
       </c>
@@ -22525,7 +22525,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="382" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="382" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A382">
         <v>2</v>
       </c>
@@ -22554,7 +22554,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="383" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="383" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A383">
         <v>2</v>
       </c>
@@ -22583,7 +22583,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="384" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="384" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A384">
         <v>2</v>
       </c>
@@ -22612,7 +22612,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="385" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="385" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A385">
         <v>2</v>
       </c>
@@ -22641,7 +22641,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="386" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="386" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A386">
         <v>2</v>
       </c>
@@ -22670,7 +22670,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="387" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="387" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A387">
         <v>2</v>
       </c>
@@ -22699,7 +22699,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="388" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="388" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A388">
         <v>2</v>
       </c>
@@ -22728,7 +22728,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="389" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="389" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A389">
         <v>2</v>
       </c>
@@ -22757,7 +22757,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="390" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="390" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A390">
         <v>2</v>
       </c>
@@ -22786,7 +22786,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="391" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="391" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A391">
         <v>2</v>
       </c>
@@ -22815,7 +22815,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="392" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="392" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A392">
         <v>2</v>
       </c>
@@ -22844,7 +22844,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="393" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="393" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A393">
         <v>2</v>
       </c>
@@ -22873,7 +22873,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="394" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="394" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A394">
         <v>2</v>
       </c>
@@ -22902,7 +22902,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="395" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="395" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A395">
         <v>2</v>
       </c>
@@ -22931,7 +22931,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="396" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="396" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A396">
         <v>2</v>
       </c>
@@ -22960,7 +22960,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="397" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="397" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A397">
         <v>2</v>
       </c>
@@ -22989,7 +22989,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="398" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="398" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A398">
         <v>2</v>
       </c>
@@ -23018,7 +23018,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="399" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="399" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A399">
         <v>2</v>
       </c>
@@ -23047,7 +23047,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="400" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="400" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A400">
         <v>2</v>
       </c>
@@ -23076,7 +23076,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="401" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="401" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A401">
         <v>2</v>
       </c>
@@ -23105,7 +23105,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="402" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="402" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A402">
         <v>2</v>
       </c>
@@ -23134,7 +23134,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="403" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="403" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A403">
         <v>2</v>
       </c>
@@ -23163,7 +23163,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="404" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="404" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A404">
         <v>2</v>
       </c>
@@ -23192,7 +23192,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="405" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="405" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A405">
         <v>2</v>
       </c>
@@ -23221,7 +23221,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="406" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="406" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A406">
         <v>2</v>
       </c>
@@ -23250,7 +23250,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="407" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="407" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A407">
         <v>2</v>
       </c>
@@ -23279,7 +23279,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="408" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="408" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A408">
         <v>2</v>
       </c>
@@ -23308,7 +23308,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="409" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="409" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A409">
         <v>2</v>
       </c>
@@ -23337,7 +23337,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="410" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="410" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A410">
         <v>2</v>
       </c>
@@ -23366,7 +23366,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="411" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="411" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A411">
         <v>2</v>
       </c>
@@ -23395,7 +23395,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="412" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="412" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A412">
         <v>2</v>
       </c>
@@ -23424,7 +23424,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="413" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="413" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A413">
         <v>2</v>
       </c>
@@ -23453,7 +23453,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="414" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="414" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A414">
         <v>2</v>
       </c>
@@ -23482,7 +23482,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="415" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="415" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A415">
         <v>2</v>
       </c>
@@ -23511,7 +23511,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="416" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="416" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A416">
         <v>2</v>
       </c>
@@ -23540,7 +23540,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="417" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
+    <row r="417" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A417">
         <v>2</v>
       </c>
@@ -23569,7 +23569,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="418" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="418" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A418">
         <v>3</v>
       </c>
@@ -23598,7 +23598,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="419" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="419" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A419">
         <v>3</v>
       </c>
@@ -23627,7 +23627,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="420" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="420" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A420">
         <v>3</v>
       </c>
@@ -23656,7 +23656,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="421" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="421" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A421">
         <v>3</v>
       </c>
@@ -23685,7 +23685,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="422" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="422" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A422">
         <v>3</v>
       </c>
@@ -23714,7 +23714,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="423" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="423" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A423">
         <v>3</v>
       </c>
@@ -23743,7 +23743,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="424" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="424" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A424">
         <v>3</v>
       </c>
@@ -23772,7 +23772,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="425" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="425" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A425">
         <v>3</v>
       </c>
@@ -23801,7 +23801,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="426" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="426" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A426">
         <v>3</v>
       </c>
@@ -23830,7 +23830,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="427" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="427" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A427">
         <v>3</v>
       </c>
@@ -23859,7 +23859,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="428" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="428" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A428">
         <v>3</v>
       </c>
@@ -23888,7 +23888,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="429" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="429" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A429">
         <v>3</v>
       </c>
@@ -23917,7 +23917,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="430" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="430" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A430">
         <v>3</v>
       </c>
@@ -23946,7 +23946,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="431" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="431" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A431">
         <v>3</v>
       </c>
@@ -23975,7 +23975,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="432" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="432" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A432">
         <v>3</v>
       </c>
@@ -24004,7 +24004,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="433" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="433" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A433">
         <v>3</v>
       </c>
@@ -24033,7 +24033,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="434" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="434" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A434">
         <v>3</v>
       </c>
@@ -24062,7 +24062,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="435" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="435" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A435">
         <v>3</v>
       </c>
@@ -24091,7 +24091,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="436" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="436" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A436">
         <v>3</v>
       </c>
@@ -24120,7 +24120,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="437" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="437" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A437">
         <v>3</v>
       </c>
@@ -24149,7 +24149,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="438" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="438" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A438">
         <v>3</v>
       </c>
@@ -24178,7 +24178,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="439" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="439" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A439">
         <v>3</v>
       </c>
@@ -24207,7 +24207,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="440" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="440" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A440">
         <v>3</v>
       </c>
@@ -24236,7 +24236,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="441" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="441" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A441">
         <v>3</v>
       </c>
@@ -24265,7 +24265,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="442" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="442" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A442">
         <v>3</v>
       </c>
@@ -24294,7 +24294,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="443" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="443" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A443">
         <v>3</v>
       </c>
@@ -24323,7 +24323,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="444" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="444" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A444">
         <v>3</v>
       </c>
@@ -24352,7 +24352,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="445" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="445" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A445">
         <v>3</v>
       </c>
@@ -24381,7 +24381,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="446" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="446" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A446">
         <v>3</v>
       </c>
@@ -24410,7 +24410,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="447" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="447" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A447">
         <v>3</v>
       </c>
@@ -24439,7 +24439,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="448" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="448" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A448">
         <v>3</v>
       </c>
@@ -24468,7 +24468,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="449" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="449" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A449">
         <v>3</v>
       </c>
@@ -24497,7 +24497,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="450" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="450" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A450">
         <v>3</v>
       </c>
@@ -24526,7 +24526,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="451" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="451" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A451">
         <v>3</v>
       </c>
@@ -24555,7 +24555,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="452" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="452" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A452">
         <v>3</v>
       </c>
@@ -24584,7 +24584,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="453" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="453" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A453">
         <v>3</v>
       </c>
@@ -24613,7 +24613,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="454" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="454" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A454">
         <v>3</v>
       </c>
@@ -24642,7 +24642,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="455" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="455" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A455">
         <v>3</v>
       </c>
@@ -24671,7 +24671,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="456" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="456" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A456">
         <v>3</v>
       </c>
@@ -24700,7 +24700,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="457" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="457" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A457">
         <v>3</v>
       </c>
@@ -24729,7 +24729,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="458" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="458" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A458">
         <v>3</v>
       </c>
@@ -24758,7 +24758,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="459" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="459" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A459">
         <v>3</v>
       </c>
@@ -24787,7 +24787,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="460" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="460" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A460">
         <v>3</v>
       </c>
@@ -24816,7 +24816,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="461" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="461" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A461">
         <v>3</v>
       </c>
@@ -24845,7 +24845,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="462" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="462" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A462">
         <v>3</v>
       </c>
@@ -24874,7 +24874,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="463" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="463" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A463">
         <v>3</v>
       </c>
@@ -24903,7 +24903,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="464" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="464" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A464">
         <v>3</v>
       </c>
@@ -24932,7 +24932,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="465" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="465" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A465">
         <v>3</v>
       </c>
@@ -24961,7 +24961,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="466" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="466" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A466">
         <v>3</v>
       </c>
@@ -24990,7 +24990,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="467" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="467" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A467">
         <v>3</v>
       </c>
@@ -25019,7 +25019,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="468" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="468" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A468">
         <v>3</v>
       </c>
@@ -25048,7 +25048,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="469" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="469" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A469">
         <v>3</v>
       </c>
@@ -25077,7 +25077,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="470" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="470" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A470">
         <v>3</v>
       </c>
@@ -25106,7 +25106,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="471" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="471" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A471">
         <v>3</v>
       </c>
@@ -25135,7 +25135,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="472" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="472" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A472">
         <v>3</v>
       </c>
@@ -25164,7 +25164,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="473" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="473" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A473">
         <v>3</v>
       </c>
@@ -25193,7 +25193,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="474" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="474" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A474">
         <v>3</v>
       </c>
@@ -25222,7 +25222,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="475" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="475" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A475">
         <v>3</v>
       </c>
@@ -25251,7 +25251,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="476" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="476" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A476">
         <v>3</v>
       </c>
@@ -25280,7 +25280,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="477" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="477" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A477">
         <v>3</v>
       </c>
@@ -25309,7 +25309,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="478" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="478" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A478">
         <v>3</v>
       </c>
@@ -25338,7 +25338,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="479" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="479" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A479">
         <v>3</v>
       </c>
@@ -25367,7 +25367,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="480" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="480" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A480">
         <v>3</v>
       </c>
@@ -25396,7 +25396,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="481" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="481" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A481">
         <v>3</v>
       </c>
@@ -25425,7 +25425,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="482" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="482" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A482">
         <v>3</v>
       </c>
@@ -25454,7 +25454,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="483" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="483" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A483">
         <v>3</v>
       </c>
@@ -25483,7 +25483,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="484" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="484" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A484">
         <v>3</v>
       </c>
@@ -25512,7 +25512,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="485" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="485" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A485">
         <v>3</v>
       </c>
@@ -25541,7 +25541,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="486" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="486" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A486">
         <v>3</v>
       </c>
@@ -25570,7 +25570,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="487" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="487" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A487">
         <v>3</v>
       </c>
@@ -25599,7 +25599,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="488" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="488" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A488">
         <v>3</v>
       </c>
@@ -25628,7 +25628,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="489" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="489" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A489">
         <v>3</v>
       </c>
@@ -25657,7 +25657,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="490" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="490" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A490">
         <v>3</v>
       </c>
@@ -25686,7 +25686,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="491" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="491" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A491">
         <v>3</v>
       </c>
@@ -25715,7 +25715,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="492" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="492" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A492">
         <v>3</v>
       </c>
@@ -25744,7 +25744,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="493" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="493" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A493">
         <v>3</v>
       </c>
@@ -25773,7 +25773,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="494" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="494" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A494">
         <v>3</v>
       </c>
@@ -25802,7 +25802,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="495" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="495" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A495">
         <v>3</v>
       </c>
@@ -25831,7 +25831,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="496" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="496" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A496">
         <v>3</v>
       </c>
@@ -25860,7 +25860,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="497" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="497" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A497">
         <v>3</v>
       </c>
@@ -25889,7 +25889,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="498" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="498" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A498">
         <v>3</v>
       </c>
@@ -25918,7 +25918,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="499" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="499" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A499">
         <v>3</v>
       </c>
@@ -25947,7 +25947,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="500" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="500" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A500">
         <v>3</v>
       </c>
@@ -25976,7 +25976,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="501" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="501" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A501">
         <v>3</v>
       </c>
@@ -26005,7 +26005,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="502" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="502" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A502">
         <v>3</v>
       </c>
@@ -26034,7 +26034,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="503" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="503" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A503">
         <v>3</v>
       </c>
@@ -26063,7 +26063,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="504" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="504" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A504">
         <v>3</v>
       </c>
@@ -26092,7 +26092,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="505" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="505" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A505">
         <v>3</v>
       </c>
@@ -26121,7 +26121,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="506" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="506" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A506">
         <v>3</v>
       </c>
@@ -26150,7 +26150,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="507" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="507" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A507">
         <v>3</v>
       </c>
@@ -26179,7 +26179,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="508" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="508" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A508">
         <v>3</v>
       </c>
@@ -26208,7 +26208,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="509" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="509" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A509">
         <v>3</v>
       </c>
@@ -26237,7 +26237,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="510" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="510" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A510">
         <v>3</v>
       </c>
@@ -26266,7 +26266,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="511" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="511" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A511">
         <v>3</v>
       </c>
@@ -26295,7 +26295,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="512" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="512" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A512">
         <v>3</v>
       </c>
@@ -26324,7 +26324,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="513" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="513" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A513">
         <v>3</v>
       </c>
@@ -26353,7 +26353,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="514" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="514" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A514">
         <v>3</v>
       </c>
@@ -26382,7 +26382,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="515" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="515" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A515">
         <v>3</v>
       </c>
@@ -26411,7 +26411,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="516" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="516" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A516">
         <v>3</v>
       </c>
@@ -26440,7 +26440,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="517" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="517" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A517">
         <v>3</v>
       </c>
@@ -26469,7 +26469,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="518" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="518" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A518">
         <v>3</v>
       </c>
@@ -26498,7 +26498,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="519" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="519" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A519">
         <v>3</v>
       </c>
@@ -26527,7 +26527,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="520" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="520" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A520">
         <v>3</v>
       </c>
@@ -26556,7 +26556,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="521" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="521" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A521">
         <v>3</v>
       </c>
@@ -26585,7 +26585,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="522" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="522" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A522">
         <v>3</v>
       </c>
@@ -26614,7 +26614,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="523" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="523" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A523">
         <v>3</v>
       </c>
@@ -26643,7 +26643,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="524" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="524" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A524">
         <v>3</v>
       </c>
@@ -26672,7 +26672,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="525" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="525" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A525">
         <v>3</v>
       </c>
@@ -26701,7 +26701,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="526" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="526" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A526">
         <v>3</v>
       </c>
@@ -26730,7 +26730,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="527" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="527" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A527">
         <v>3</v>
       </c>
@@ -26759,7 +26759,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="528" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="528" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A528">
         <v>3</v>
       </c>
@@ -26788,7 +26788,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="529" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="529" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A529">
         <v>3</v>
       </c>
@@ -26817,7 +26817,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="530" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="530" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A530">
         <v>3</v>
       </c>
@@ -26846,7 +26846,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="531" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="531" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A531">
         <v>3</v>
       </c>
@@ -26875,7 +26875,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="532" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="532" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A532">
         <v>3</v>
       </c>
@@ -26904,7 +26904,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="533" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="533" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A533">
         <v>3</v>
       </c>
@@ -26933,7 +26933,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="534" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="534" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A534">
         <v>3</v>
       </c>
@@ -26962,7 +26962,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="535" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="535" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A535">
         <v>3</v>
       </c>
@@ -26991,7 +26991,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="536" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="536" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A536">
         <v>3</v>
       </c>
@@ -27020,7 +27020,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="537" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="537" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A537">
         <v>3</v>
       </c>
@@ -27049,7 +27049,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="538" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="538" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A538">
         <v>3</v>
       </c>
@@ -27078,7 +27078,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="539" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="539" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A539">
         <v>3</v>
       </c>
@@ -27107,7 +27107,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="540" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="540" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A540">
         <v>3</v>
       </c>
@@ -27136,7 +27136,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="541" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="541" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A541">
         <v>3</v>
       </c>
@@ -27165,7 +27165,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="542" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="542" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A542">
         <v>3</v>
       </c>
@@ -27194,7 +27194,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="543" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="543" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A543">
         <v>3</v>
       </c>
@@ -27223,7 +27223,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="544" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="544" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A544">
         <v>3</v>
       </c>
@@ -27252,7 +27252,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="545" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="545" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A545">
         <v>3</v>
       </c>
@@ -27281,7 +27281,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="546" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="546" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A546">
         <v>3</v>
       </c>
@@ -27310,7 +27310,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="547" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="547" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A547">
         <v>3</v>
       </c>
@@ -27339,7 +27339,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="548" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="548" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A548">
         <v>3</v>
       </c>
@@ -27368,7 +27368,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="549" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="549" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A549">
         <v>3</v>
       </c>
@@ -27397,7 +27397,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="550" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="550" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A550">
         <v>3</v>
       </c>
@@ -27426,7 +27426,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="551" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="551" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A551">
         <v>3</v>
       </c>
@@ -27455,7 +27455,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="552" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="552" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A552">
         <v>3</v>
       </c>
@@ -27484,7 +27484,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="553" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="553" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A553">
         <v>3</v>
       </c>
@@ -27513,7 +27513,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="554" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="554" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A554">
         <v>3</v>
       </c>
@@ -27542,7 +27542,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="555" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="555" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A555">
         <v>3</v>
       </c>
@@ -27571,7 +27571,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="556" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="556" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A556">
         <v>3</v>
       </c>
@@ -27600,7 +27600,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="557" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="557" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A557">
         <v>3</v>
       </c>
@@ -27629,7 +27629,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="558" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="558" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A558">
         <v>3</v>
       </c>
@@ -27658,7 +27658,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="559" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="559" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A559">
         <v>3</v>
       </c>
@@ -27687,7 +27687,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="560" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="560" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A560">
         <v>3</v>
       </c>
@@ -27720,7 +27720,7 @@
   <autoFilter ref="A1:I560" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="0">
       <filters>
-        <filter val="3"/>
+        <filter val="2"/>
       </filters>
     </filterColumn>
   </autoFilter>
@@ -31088,7 +31088,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF13226B-0231-40BE-8C56-E7B91CEF9201}">
   <dimension ref="A1:Y29"/>
   <sheetViews>
-    <sheetView topLeftCell="K13" workbookViewId="0">
+    <sheetView topLeftCell="K1" workbookViewId="0">
       <selection activeCell="X18" activeCellId="1" sqref="S18:S29 X18:Y29"/>
     </sheetView>
   </sheetViews>
@@ -31864,7 +31864,7 @@
         <v>-0.50465946628012959</v>
       </c>
       <c r="G18" s="9">
-        <f>MIN((I$5*(C18-N$5)/(C18+M$5)),((L$5/4)*((C18-N$5)/(C18+2*N$5))))</f>
+        <f t="shared" ref="G18:G29" si="6">MIN((I$5*(C18-N$5)/(C18+M$5)),((L$5/4)*((C18-N$5)/(C18+2*N$5))))</f>
         <v>-0.41795517688365058</v>
       </c>
       <c r="H18" s="1">
@@ -31949,75 +31949,75 @@
         <v>0.41428264142826421</v>
       </c>
       <c r="F19" s="9">
-        <f>MIN((I$5*(C19-N$4)/(C19+M$5)),((L$4/4)*((C19-N$4)/(C19+2*N$4))))</f>
+        <f t="shared" ref="F19:F29" si="7">MIN((I$5*(C19-N$4)/(C19+M$5)),((L$4/4)*((C19-N$4)/(C19+2*N$4))))</f>
         <v>0.26917874396135261</v>
       </c>
       <c r="G19" s="9">
-        <f>MIN((I$5*(C19-N$5)/(C19+M$5)),((L$5/4)*((C19-N$5)/(C19+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>0.23457004830917877</v>
       </c>
       <c r="H19" s="1">
-        <f t="shared" ref="H19:H29" si="6">AVERAGE(D19:G19)</f>
+        <f t="shared" ref="H19:H29" si="8">AVERAGE(D19:G19)</f>
         <v>0.3661001505139484</v>
       </c>
       <c r="I19">
-        <f t="shared" ref="I19:I29" si="7">STDEV(D19:G19)/SQRT(COUNTA(D19:G19))</f>
+        <f t="shared" ref="I19:I29" si="9">STDEV(D19:G19)/SQRT(COUNTA(D19:G19))</f>
         <v>7.1596320936051117E-2</v>
       </c>
       <c r="K19" s="1">
-        <f t="shared" ref="K19:K29" si="8">C19-10</f>
+        <f t="shared" ref="K19:K29" si="10">C19-10</f>
         <v>30</v>
       </c>
       <c r="L19" s="8">
-        <f t="shared" ref="L19:L29" si="9">MIN((I$6*(K19-N$6)/(K19+M$6)),((L$6/4)*((K19-N$6)/(K19+2*N$6))))</f>
+        <f t="shared" ref="L19:L29" si="11">MIN((I$6*(K19-N$6)/(K19+M$6)),((L$6/4)*((K19-N$6)/(K19+2*N$6))))</f>
         <v>-2.6829316760692876</v>
       </c>
       <c r="M19" s="9">
-        <f t="shared" ref="M19:M29" si="10">MIN((I$7*(K19-N$7)/(K19+M$7)),((L$7/4)*((K19-N$7)/(K19+2*N$7))))</f>
+        <f t="shared" ref="M19:M29" si="12">MIN((I$7*(K19-N$7)/(K19+M$7)),((L$7/4)*((K19-N$7)/(K19+2*N$7))))</f>
         <v>-0.44857252296757499</v>
       </c>
       <c r="N19" s="9">
-        <f t="shared" ref="N19:O29" si="11">MIN((I$8*(K19-N$8)/(K19+M$8)),((L$8/4)*((K19-N$8)/(K19+2*N$8))))</f>
+        <f t="shared" ref="N19:N29" si="13">MIN((I$8*(K19-N$8)/(K19+M$8)),((L$8/4)*((K19-N$8)/(K19+2*N$8))))</f>
         <v>-0.30407736889655501</v>
       </c>
       <c r="O19" s="9">
-        <f t="shared" ref="O19:O29" si="12">MIN((I$9*(K19-N$9)/(K19+M$9)),((L$9/4)*((K19-N$9)/(K19+2*N$9))))</f>
+        <f t="shared" ref="O19:O29" si="14">MIN((I$9*(K19-N$9)/(K19+M$9)),((L$9/4)*((K19-N$9)/(K19+2*N$9))))</f>
         <v>-0.32293051766213254</v>
       </c>
       <c r="P19" s="1">
-        <f t="shared" ref="P19:P29" si="13">AVERAGE(L19:O19)</f>
+        <f t="shared" ref="P19:P29" si="15">AVERAGE(L19:O19)</f>
         <v>-0.93962802139888757</v>
       </c>
       <c r="Q19">
-        <f t="shared" ref="Q19:Q29" si="14">STDEV(L19:O19)/SQRT(COUNTA(L19:O19))</f>
+        <f t="shared" ref="Q19:Q29" si="16">STDEV(L19:O19)/SQRT(COUNTA(L19:O19))</f>
         <v>0.58198536478864615</v>
       </c>
       <c r="S19" s="1">
-        <f t="shared" ref="S19:S29" si="15">K19-10</f>
+        <f t="shared" ref="S19:S29" si="17">K19-10</f>
         <v>20</v>
       </c>
       <c r="T19" s="8">
-        <f t="shared" ref="T19:T29" si="16">MIN((I$10*(S19-N$10)/(S19+M$10)),((L$10/4)*((S19-N$10)/(S19+2*N$10))))</f>
+        <f t="shared" ref="T19:T29" si="18">MIN((I$10*(S19-N$10)/(S19+M$10)),((L$10/4)*((S19-N$10)/(S19+2*N$10))))</f>
         <v>-1.8430169756743007</v>
       </c>
       <c r="U19" s="9">
-        <f t="shared" ref="U19:U29" si="17">MIN((I$11*(S19-N$11)/(S19+M$11)),((L$11/4)*((S19-N$11)/(S19+2*N$11))))</f>
+        <f t="shared" ref="U19:U29" si="19">MIN((I$11*(S19-N$11)/(S19+M$11)),((L$11/4)*((S19-N$11)/(S19+2*N$11))))</f>
         <v>-2.3382184206762853</v>
       </c>
       <c r="V19" s="9">
-        <f t="shared" ref="V19:V29" si="18">MIN((I$12*(S19-N$12)/(S19+M$12)),((L$12/4)*((S19-N$12)/(S19+2*N$12))))</f>
+        <f t="shared" ref="V19:V29" si="20">MIN((I$12*(S19-N$12)/(S19+M$12)),((L$12/4)*((S19-N$12)/(S19+2*N$12))))</f>
         <v>-1.7266730000131034</v>
       </c>
       <c r="W19" s="9">
-        <f t="shared" ref="W19:W29" si="19">MIN((I$13*(S19-N$13)/(S19+M$13)),((L$13/4)*((S19-N$13)/(S19+2*N$13))))</f>
+        <f t="shared" ref="W19:W29" si="21">MIN((I$13*(S19-N$13)/(S19+M$13)),((L$13/4)*((S19-N$13)/(S19+2*N$13))))</f>
         <v>-1.9247562206082196</v>
       </c>
       <c r="X19" s="1">
-        <f t="shared" ref="X19:X29" si="20">AVERAGE(T19:W19)</f>
+        <f t="shared" ref="X19:X29" si="22">AVERAGE(T19:W19)</f>
         <v>-1.9581661542429774</v>
       </c>
       <c r="Y19">
-        <f t="shared" ref="Y19:Y29" si="21">STDEV(T19:W19)/SQRT(COUNTA(T19:W19))</f>
+        <f t="shared" ref="Y19:Y29" si="23">STDEV(T19:W19)/SQRT(COUNTA(T19:W19))</f>
         <v>0.13304271327500605</v>
       </c>
     </row>
@@ -32038,75 +32038,75 @@
         <v>1.021998887588945</v>
       </c>
       <c r="F20" s="9">
-        <f>MIN((I$5*(C20-N$4)/(C20+M$5)),((L$4/4)*((C20-N$4)/(C20+2*N$4))))</f>
+        <f t="shared" si="7"/>
         <v>0.64132701421800942</v>
       </c>
       <c r="G20" s="9">
-        <f>MIN((I$5*(C20-N$5)/(C20+M$5)),((L$5/4)*((C20-N$5)/(C20+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>0.60737440758293837</v>
       </c>
       <c r="H20" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>0.88246632983256257</v>
       </c>
       <c r="I20">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.15684253395551478</v>
       </c>
       <c r="K20" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>40</v>
       </c>
       <c r="L20" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>0.89680754580083433</v>
       </c>
       <c r="M20" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>0.65013544488435093</v>
       </c>
       <c r="N20" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>0.31324582338902146</v>
       </c>
       <c r="O20" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>0.45</v>
       </c>
       <c r="P20" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>0.57754720351855171</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>0.12692508538588057</v>
       </c>
       <c r="S20" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>30</v>
       </c>
       <c r="T20" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>-0.38100831708651411</v>
       </c>
       <c r="U20" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>-0.44499447286975541</v>
       </c>
       <c r="V20" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>-0.37516546511035398</v>
       </c>
       <c r="W20" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>-0.54529798141292318</v>
       </c>
       <c r="X20" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>-0.43661655911988662</v>
       </c>
       <c r="Y20">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>3.9528844455081501E-2</v>
       </c>
     </row>
@@ -32127,75 +32127,75 @@
         <v>3.741507551759744</v>
       </c>
       <c r="F21" s="9">
-        <f>MIN((I$5*(C21-N$4)/(C21+M$5)),((L$4/4)*((C21-N$4)/(C21+2*N$4))))</f>
+        <f t="shared" si="7"/>
         <v>2.3087445887445885</v>
       </c>
       <c r="G21" s="9">
-        <f>MIN((I$5*(C21-N$5)/(C21+M$5)),((L$5/4)*((C21-N$5)/(C21+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>2.2777316017316016</v>
       </c>
       <c r="H21" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>3.1911098596096164</v>
       </c>
       <c r="I21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>0.53748272727568402</v>
       </c>
       <c r="K21" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>90</v>
       </c>
       <c r="L21" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>9.21238982205222</v>
       </c>
       <c r="M21" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>4.2687299490469899</v>
       </c>
       <c r="N21" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>2.3200072358900146</v>
       </c>
       <c r="O21" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>2.9547169811320755</v>
       </c>
       <c r="P21" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>4.6889609970303248</v>
       </c>
       <c r="Q21">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>1.5614508930753006</v>
       </c>
       <c r="S21" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>80</v>
       </c>
       <c r="T21" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>2.0632888238522038</v>
       </c>
       <c r="U21" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>3.9132762312633824</v>
       </c>
       <c r="V21" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>1.8299287410926366</v>
       </c>
       <c r="W21" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>2.1823914541695379</v>
       </c>
       <c r="X21" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>2.4972213125944402</v>
       </c>
       <c r="Y21">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.47765975976716157</v>
       </c>
     </row>
@@ -32216,75 +32216,75 @@
         <v>7.9653554565900588</v>
       </c>
       <c r="F22" s="9">
-        <f>MIN((I$5*(C22-N$4)/(C22+M$5)),((L$4/4)*((C22-N$4)/(C22+2*N$4))))</f>
+        <f t="shared" si="7"/>
         <v>4.9052398523985232</v>
       </c>
       <c r="G22" s="9">
-        <f>MIN((I$5*(C22-N$5)/(C22+M$5)),((L$5/4)*((C22-N$5)/(C22+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>4.8788044280442806</v>
       </c>
       <c r="H22" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>6.7701830123592872</v>
       </c>
       <c r="I22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.1196446180097892</v>
       </c>
       <c r="K22" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>190</v>
       </c>
       <c r="L22" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>22.286339654926568</v>
       </c>
       <c r="M22" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>9.7825051595491352</v>
       </c>
       <c r="N22" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>5.4113051470588243</v>
       </c>
       <c r="O22" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>6.7714285714285714</v>
       </c>
       <c r="P22" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>11.062894633240775</v>
       </c>
       <c r="Q22">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>3.8509983558287875</v>
       </c>
       <c r="S22" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>180</v>
       </c>
       <c r="T22" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>5.4553888974795113</v>
       </c>
       <c r="U22" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>9.4377271128684885</v>
       </c>
       <c r="V22" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>4.8532674185076479</v>
       </c>
       <c r="W22" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>5.962169312169312</v>
       </c>
       <c r="X22" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>6.4271381852562399</v>
       </c>
       <c r="Y22">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>1.028802200486953</v>
       </c>
     </row>
@@ -32305,75 +32305,75 @@
         <v>11.094076926068526</v>
       </c>
       <c r="F23" s="9">
-        <f>MIN((I$5*(C23-N$4)/(C23+M$5)),((L$4/4)*((C23-N$4)/(C23+2*N$4))))</f>
+        <f t="shared" si="7"/>
         <v>6.8338263665594843</v>
       </c>
       <c r="G23" s="9">
-        <f>MIN((I$5*(C23-N$5)/(C23+M$5)),((L$5/4)*((C23-N$5)/(C23+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>6.8107909967845659</v>
       </c>
       <c r="H23" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>9.3867478607342889</v>
       </c>
       <c r="I23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.521373667136549</v>
       </c>
       <c r="K23" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>290</v>
       </c>
       <c r="L23" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>32.097104704854615</v>
       </c>
       <c r="M23" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>13.785450061652282</v>
       </c>
       <c r="N23" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.0245288814754732</v>
       </c>
       <c r="O23" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>9.5424657534246577</v>
       </c>
       <c r="P23" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>15.612387350351758</v>
       </c>
       <c r="Q23">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>5.6692067889386744</v>
       </c>
       <c r="S23" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>280</v>
       </c>
       <c r="T23" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>7.9389312977099236</v>
       </c>
       <c r="U23" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>11.25747549981971</v>
       </c>
       <c r="V23" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>7.0674695570721262</v>
       </c>
       <c r="W23" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>8.263957097067923</v>
       </c>
       <c r="X23" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>8.6319583629174197</v>
       </c>
       <c r="Y23">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.91089136310538588</v>
       </c>
     </row>
@@ -32394,75 +32394,75 @@
         <v>12.812581571435196</v>
       </c>
       <c r="F24" s="9">
-        <f>MIN((I$5*(C24-N$4)/(C24+M$5)),((L$4/4)*((C24-N$4)/(C24+2*N$4))))</f>
+        <f t="shared" si="7"/>
         <v>8.3228490028490025</v>
       </c>
       <c r="G24" s="9">
-        <f>MIN((I$5*(C24-N$5)/(C24+M$5)),((L$5/4)*((C24-N$5)/(C24+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>8.202447663994489</v>
       </c>
       <c r="H24" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10.788293656626953</v>
       </c>
       <c r="I24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.4726819055049818</v>
       </c>
       <c r="K24" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>390</v>
       </c>
       <c r="L24" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>39.730844335959169</v>
       </c>
       <c r="M24" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>16.62484861553396</v>
       </c>
       <c r="N24" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.6179382944610632</v>
       </c>
       <c r="O24" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>11.64578313253012</v>
       </c>
       <c r="P24" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>18.904853594621077</v>
       </c>
       <c r="Q24">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>7.1822052905633251</v>
       </c>
       <c r="S24" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>380</v>
       </c>
       <c r="T24" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9.4859111052211951</v>
       </c>
       <c r="U24" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>12.26009394202409</v>
       </c>
       <c r="V24" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>8.7590227782367513</v>
       </c>
       <c r="W24" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>9.0421210363246445</v>
       </c>
       <c r="X24" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>9.8867872154516689</v>
       </c>
       <c r="Y24">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.80511904162030701</v>
       </c>
     </row>
@@ -32483,75 +32483,75 @@
         <v>13.430430165381999</v>
       </c>
       <c r="F25" s="9">
-        <f>MIN((I$5*(C25-N$4)/(C25+M$5)),((L$4/4)*((C25-N$4)/(C25+2*N$4))))</f>
+        <f t="shared" si="7"/>
         <v>9.5072122762148332</v>
       </c>
       <c r="G25" s="9">
-        <f>MIN((I$5*(C25-N$5)/(C25+M$5)),((L$5/4)*((C25-N$5)/(C25+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>8.6037477971960747</v>
       </c>
       <c r="H25" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>11.501838022871087</v>
       </c>
       <c r="I25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.4399929558867284</v>
       </c>
       <c r="K25" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>490</v>
       </c>
       <c r="L25" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>42.8035698274008</v>
       </c>
       <c r="M25" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>17.429552580144438</v>
       </c>
       <c r="N25" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>7.9978910840705408</v>
       </c>
       <c r="O25" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>12.547657623095784</v>
       </c>
       <c r="P25" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>20.194667778677893</v>
       </c>
       <c r="Q25">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>7.7784233619223908</v>
       </c>
       <c r="S25" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>480</v>
       </c>
       <c r="T25" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>9.9815805267499957</v>
       </c>
       <c r="U25" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>12.895048855734013</v>
       </c>
       <c r="V25" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>9.2417109911522584</v>
       </c>
       <c r="W25" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>9.5369040800035361</v>
       </c>
       <c r="X25" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>10.413811113409951</v>
       </c>
       <c r="Y25">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.84093938821474701</v>
       </c>
     </row>
@@ -32572,75 +32572,75 @@
         <v>13.862961244647694</v>
       </c>
       <c r="F26" s="9">
-        <f>MIN((I$5*(C26-N$4)/(C26+M$5)),((L$4/4)*((C26-N$4)/(C26+2*N$4))))</f>
+        <f t="shared" si="7"/>
         <v>10.471740139211136</v>
       </c>
       <c r="G26" s="9">
-        <f>MIN((I$5*(C26-N$5)/(C26+M$5)),((L$5/4)*((C26-N$5)/(C26+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>8.8848622061683731</v>
       </c>
       <c r="H26" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>12.035140220446598</v>
       </c>
       <c r="I26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.4153201084857221</v>
       </c>
       <c r="K26" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>590</v>
       </c>
       <c r="L26" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>44.304349383875028</v>
       </c>
       <c r="M26" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>17.9881697054245</v>
       </c>
       <c r="N26" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.2620046085551788</v>
       </c>
       <c r="O26" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>12.949810024781479</v>
       </c>
       <c r="P26" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>20.876083430659047</v>
       </c>
       <c r="Q26">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>8.0579385592407604</v>
       </c>
       <c r="S26" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>580</v>
       </c>
       <c r="T26" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>10.323791923037684</v>
       </c>
       <c r="U26" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>13.333240548585575</v>
       </c>
       <c r="V26" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>9.5604221058331262</v>
       </c>
       <c r="W26" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>9.8792585828078465</v>
       </c>
       <c r="X26" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>10.774178290066057</v>
       </c>
       <c r="Y26">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.86726259382548576</v>
       </c>
     </row>
@@ -32661,75 +32661,75 @@
         <v>14.18267774924837</v>
       </c>
       <c r="F27" s="9">
-        <f>MIN((I$5*(C27-N$4)/(C27+M$5)),((L$4/4)*((C27-N$4)/(C27+2*N$4))))</f>
+        <f t="shared" si="7"/>
         <v>11.272441613588109</v>
       </c>
       <c r="G27" s="9">
-        <f>MIN((I$5*(C27-N$5)/(C27+M$5)),((L$5/4)*((C27-N$5)/(C27+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>9.092750668547211</v>
       </c>
       <c r="H27" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>12.451242585543005</v>
       </c>
       <c r="I27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.4005875251848829</v>
       </c>
       <c r="K27" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>690</v>
       </c>
       <c r="L27" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>45.410290856562298</v>
       </c>
       <c r="M27" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>18.398612526916743</v>
       </c>
       <c r="N27" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.4562468302661014</v>
       </c>
       <c r="O27" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>13.24529070188211</v>
       </c>
       <c r="P27" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>21.377610228906814</v>
       </c>
       <c r="Q27">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>8.2640810057173972</v>
       </c>
       <c r="S27" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>680</v>
       </c>
       <c r="T27" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>10.574257636674515</v>
       </c>
       <c r="U27" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>13.653860013679811</v>
       </c>
       <c r="V27" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>9.7937336721000463</v>
       </c>
       <c r="W27" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10.130221066710847</v>
       </c>
       <c r="X27" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>11.038018097291305</v>
       </c>
       <c r="Y27">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.88647437807826079</v>
       </c>
     </row>
@@ -32749,75 +32749,75 @@
         <v>14.428624871153918</v>
       </c>
       <c r="F28" s="9">
-        <f>MIN((I$5*(C28-N$4)/(C28+M$5)),((L$4/4)*((C28-N$4)/(C28+2*N$4))))</f>
+        <f t="shared" si="7"/>
         <v>11.947788649706457</v>
       </c>
       <c r="G28" s="9">
-        <f>MIN((I$5*(C28-N$5)/(C28+M$5)),((L$5/4)*((C28-N$5)/(C28+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>9.2527275240168905</v>
       </c>
       <c r="H28" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>12.786162664464879</v>
       </c>
       <c r="I28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.394484724015705</v>
       </c>
       <c r="K28" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>790</v>
       </c>
       <c r="L28" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>46.259096436971653</v>
       </c>
       <c r="M28" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>18.712932907778487</v>
       </c>
       <c r="N28" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.6051053553155938</v>
       </c>
       <c r="O28" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>13.471572157179313</v>
       </c>
       <c r="P28" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>21.762176714311259</v>
       </c>
       <c r="Q28">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>8.4223888849828317</v>
       </c>
       <c r="S28" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>780</v>
       </c>
       <c r="T28" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>10.765511597678527</v>
       </c>
       <c r="U28" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>13.898629120341534</v>
       </c>
       <c r="V28" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>9.9719149060732679</v>
       </c>
       <c r="W28" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10.322077925577814</v>
       </c>
       <c r="X28" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>11.239533387417787</v>
       </c>
       <c r="Y28">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.90111356631239925</v>
       </c>
     </row>
@@ -32837,75 +32837,75 @@
         <v>14.782191149888778</v>
       </c>
       <c r="F29" s="9">
-        <f>MIN((I$5*(C29-N$4)/(C29+M$5)),((L$4/4)*((C29-N$4)/(C29+2*N$4))))</f>
+        <f t="shared" si="7"/>
         <v>13.024230118443317</v>
       </c>
       <c r="G29" s="9">
-        <f>MIN((I$5*(C29-N$5)/(C29+M$5)),((L$5/4)*((C29-N$5)/(C29+2*N$5))))</f>
+        <f t="shared" si="6"/>
         <v>9.4827897634430371</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>13.293995969506465</v>
       </c>
       <c r="I29">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1.4004547828898559</v>
       </c>
       <c r="K29" s="1">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>990</v>
       </c>
       <c r="L29" s="8">
-        <f t="shared" si="9"/>
+        <f t="shared" si="11"/>
         <v>47.47634224385186</v>
       </c>
       <c r="M29" s="9">
-        <f t="shared" si="10"/>
+        <f t="shared" si="12"/>
         <v>19.162643661421285</v>
       </c>
       <c r="N29" s="9">
-        <f t="shared" si="11"/>
+        <f t="shared" si="13"/>
         <v>8.8182436980000958</v>
       </c>
       <c r="O29" s="9">
-        <f t="shared" si="12"/>
+        <f t="shared" si="14"/>
         <v>13.795322095118767</v>
       </c>
       <c r="P29" s="1">
-        <f t="shared" si="13"/>
+        <f t="shared" si="15"/>
         <v>22.313137924598003</v>
       </c>
       <c r="Q29">
-        <f t="shared" si="14"/>
+        <f t="shared" si="16"/>
         <v>8.6495559732220659</v>
       </c>
       <c r="S29" s="1">
-        <f t="shared" si="15"/>
+        <f t="shared" si="17"/>
         <v>980</v>
       </c>
       <c r="T29" s="8">
-        <f t="shared" si="16"/>
+        <f t="shared" si="18"/>
         <v>11.038313614712928</v>
       </c>
       <c r="U29" s="9">
-        <f t="shared" si="17"/>
+        <f t="shared" si="19"/>
         <v>14.247683821136725</v>
       </c>
       <c r="V29" s="9">
-        <f t="shared" si="18"/>
+        <f t="shared" si="20"/>
         <v>10.226109235273599</v>
       </c>
       <c r="W29" s="9">
-        <f t="shared" si="19"/>
+        <f t="shared" si="21"/>
         <v>10.596075559323774</v>
       </c>
       <c r="X29" s="1">
-        <f t="shared" si="20"/>
+        <f t="shared" si="22"/>
         <v>11.527045557611755</v>
       </c>
       <c r="Y29">
-        <f t="shared" si="21"/>
+        <f t="shared" si="23"/>
         <v>0.92194865753002786</v>
       </c>
     </row>
@@ -32920,9 +32920,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5D6A822-69BB-4753-9C8F-1786BE545752}">
   <dimension ref="A1:AI35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A11" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A22" sqref="A22:AI35"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -35507,7 +35507,7 @@
   <dimension ref="A1:G120"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:N1048576"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -38281,7 +38281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31B047C8-F96B-4ACF-9367-0CC8121300C3}">
   <dimension ref="A1:D37"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -38860,7 +38860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="E7:E18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>